<commit_message>
Fiksa bruleveranse, skal ha lengde bru, ikke lengde høydebegrensning
</commit_message>
<xml_diff>
--- a/kostraleveranse2020/Kostra 19 - Bruer hoyde mindre enn 4m.xlsx
+++ b/kostraleveranse2020/Kostra 19 - Bruer hoyde mindre enn 4m.xlsx
@@ -447,7 +447,7 @@
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>Lengde (m)</t>
+          <t>Lengde</t>
         </is>
       </c>
     </row>
@@ -459,7 +459,7 @@
         <v>1</v>
       </c>
       <c r="C2" t="n">
-        <v>126.561</v>
+        <v>118.8</v>
       </c>
     </row>
     <row r="3">
@@ -470,7 +470,7 @@
         <v>4</v>
       </c>
       <c r="C3" t="n">
-        <v>414.727</v>
+        <v>412.34</v>
       </c>
     </row>
     <row r="4">
@@ -481,7 +481,7 @@
         <v>1</v>
       </c>
       <c r="C4" t="n">
-        <v>79</v>
+        <v>81</v>
       </c>
     </row>
     <row r="5">
@@ -492,7 +492,7 @@
         <v>5</v>
       </c>
       <c r="C5" t="n">
-        <v>196.481</v>
+        <v>261.25</v>
       </c>
     </row>
     <row r="6">
@@ -503,7 +503,7 @@
         <v>2</v>
       </c>
       <c r="C6" t="n">
-        <v>29.098</v>
+        <v>159.82</v>
       </c>
     </row>
     <row r="7">
@@ -514,7 +514,7 @@
         <v>2</v>
       </c>
       <c r="C7" t="n">
-        <v>152.091</v>
+        <v>203</v>
       </c>
     </row>
     <row r="8">
@@ -525,7 +525,7 @@
         <v>2</v>
       </c>
       <c r="C8" t="n">
-        <v>1.964</v>
+        <v>136.18</v>
       </c>
     </row>
   </sheetData>
@@ -539,7 +539,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B7"/>
+  <dimension ref="A1:B9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -607,7 +607,7 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>60</t>
+          <t>60(1263=7304)</t>
         </is>
       </c>
     </row>
@@ -632,6 +632,30 @@
       <c r="B7" t="inlineStr">
         <is>
           <t>2020-12-31</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>egenskapfilter_bru</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>1263=7304</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>overlapp fra søk etter høydebegrensning</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>0.80121169-0.80129544@1125844,0.03534597-0.06032389@121713,0.97659909-0.97806091@22107,0.47770288-0.53110961@1175773,0.97700648-0.97727196@181212,0.93980412-0.94078725@22110,0.73952864-0.88387233@1060365,0.95303187-0.9588474@22110,0.87978719-0.88356741@384326,0.01180717-0.01196701@72561,0.48914175-0.88487916@1060530,0.60680381-0.60690384@805106,0.91324653-0.97386356@121475,0.96427989-0.97700648@181212,0.08871395-0.78240909@705367,0.94078725-0.95303187@22110,0.61378309-0.9735731@72630,0.21997673-0.22009309@1126325,0.98037222-0.99155114@22110,0.00109324-0.01185904@705136</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Kjørte rapport 19 på ny, bedre metode. Samme tall, men penere
</commit_message>
<xml_diff>
--- a/kostraleveranse2020/Kostra 19 - Bruer hoyde mindre enn 4m.xlsx
+++ b/kostraleveranse2020/Kostra 19 - Bruer hoyde mindre enn 4m.xlsx
@@ -539,7 +539,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B9"/>
+  <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -583,31 +583,31 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>2021-02-03</t>
+          <t>2021-02-04</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>egenskap</t>
+          <t>overlapp</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t xml:space="preserve"> 5277 &lt; 4 AND ( 5270=8168 OR 5270=8149 ) </t>
+          <t>591(5277 &lt; 4 AND (5270=8168 OR 5270=8149))</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>overlapp</t>
+          <t>egenskap</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>60(1263=7304)</t>
+          <t>1263=7304</t>
         </is>
       </c>
     </row>
@@ -632,30 +632,6 @@
       <c r="B7" t="inlineStr">
         <is>
           <t>2020-12-31</t>
-        </is>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="inlineStr">
-        <is>
-          <t>egenskapfilter_bru</t>
-        </is>
-      </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>1263=7304</t>
-        </is>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="inlineStr">
-        <is>
-          <t>overlapp fra søk etter høydebegrensning</t>
-        </is>
-      </c>
-      <c r="B9" t="inlineStr">
-        <is>
-          <t>0.80121169-0.80129544@1125844,0.03534597-0.06032389@121713,0.97659909-0.97806091@22107,0.47770288-0.53110961@1175773,0.97700648-0.97727196@181212,0.93980412-0.94078725@22110,0.73952864-0.88387233@1060365,0.95303187-0.9588474@22110,0.87978719-0.88356741@384326,0.01180717-0.01196701@72561,0.48914175-0.88487916@1060530,0.60680381-0.60690384@805106,0.91324653-0.97386356@121475,0.96427989-0.97700648@181212,0.08871395-0.78240909@705367,0.94078725-0.95303187@22110,0.61378309-0.9735731@72630,0.21997673-0.22009309@1126325,0.98037222-0.99155114@22110,0.00109324-0.01185904@705136</t>
         </is>
       </c>
     </row>

</xml_diff>